<commit_message>
Sixth commit - optimized to main branch added ajx loader for userSettings
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="349" documentId="13_ncr:1_{C7C6B02C-8938-4D98-A054-40F955FDA2A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F4F8DEEB-1014-463E-BD39-517A58859F87}"/>
+  <xr:revisionPtr revIDLastSave="350" documentId="13_ncr:1_{C7C6B02C-8938-4D98-A054-40F955FDA2A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{44BEDD29-AF11-4250-936A-8425AFC394C4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -1049,14 +1049,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
@@ -3187,7 +3187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAEAB4E-6506-4FC5-8483-B6EF264C5C31}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Seventh commit - updated and optimized the framework
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="350" documentId="13_ncr:1_{C7C6B02C-8938-4D98-A054-40F955FDA2A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{44BEDD29-AF11-4250-936A-8425AFC394C4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{B371B182-6664-4089-A8A7-BBAE6E88EEEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,8 @@
     <sheet name="Application Command" sheetId="16" r:id="rId15"/>
     <sheet name="Environment Variable" sheetId="17" r:id="rId16"/>
     <sheet name="History Cleaner" sheetId="18" r:id="rId17"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId18"/>
+    <sheet name="Sheet2" sheetId="19" r:id="rId18"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId19"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="215">
   <si>
     <t>Email</t>
   </si>
@@ -681,6 +682,12 @@
   </si>
   <si>
     <t>Clear The Command Dialogue Last Visited Folder History</t>
+  </si>
+  <si>
+    <t>Forcefully Close The Browser Instance</t>
+  </si>
+  <si>
+    <t>Internet Explorer</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2017,7 +2024,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,10 +2063,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47979A52-AC7D-48A2-A130-CC6D77928906}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,22 +2074,23 @@
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -2093,46 +2101,49 @@
         <v>196</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -2152,7 +2163,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>32</v>
@@ -2181,63 +2192,135 @@
       <c r="P2" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C36428-63BD-472E-9AEF-E7AD7E6DF397}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
   <dimension ref="A1:K28"/>
   <sheetViews>
@@ -3503,7 +3586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145BBCDE-DFF0-4BEB-8420-1E3DF9A8E932}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
@@ -3868,7 +3951,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3914,4 +3997,251 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
+    <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceDateTaken" ma:index="8" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="11" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="13" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="14" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
11th commit - added new test cases task manager tc18,19
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{B371B182-6664-4089-A8A7-BBAE6E88EEEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{70064AC4-793D-43B6-A904-992B3B16F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BDA10CFC-3358-4D3C-832B-E238CCB56768}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,9 @@
     <sheet name="Application Command" sheetId="16" r:id="rId15"/>
     <sheet name="Environment Variable" sheetId="17" r:id="rId16"/>
     <sheet name="History Cleaner" sheetId="18" r:id="rId17"/>
-    <sheet name="Sheet2" sheetId="19" r:id="rId18"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId19"/>
+    <sheet name="Registry Backup Restore" sheetId="19" r:id="rId18"/>
+    <sheet name="Startup Application List" sheetId="20" r:id="rId19"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="231">
   <si>
     <t>Email</t>
   </si>
@@ -688,6 +689,54 @@
   </si>
   <si>
     <t>Internet Explorer</t>
+  </si>
+  <si>
+    <t>Obtain Registry</t>
+  </si>
+  <si>
+    <t>Registry Key User</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Backup Path</t>
+  </si>
+  <si>
+    <t>Backup Name</t>
+  </si>
+  <si>
+    <t>HKEY_USERS</t>
+  </si>
+  <si>
+    <t>xxxxxx</t>
+  </si>
+  <si>
+    <t>C:\abc</t>
+  </si>
+  <si>
+    <t>demo backup</t>
+  </si>
+  <si>
+    <t>Registry Backup</t>
+  </si>
+  <si>
+    <t>Application Name</t>
+  </si>
+  <si>
+    <t>isEnabled</t>
+  </si>
+  <si>
+    <t>C:\Example\file.exe</t>
+  </si>
+  <si>
+    <t>file.exe</t>
+  </si>
+  <si>
+    <t>C:\file.exe</t>
+  </si>
+  <si>
+    <t>file1.exe</t>
   </si>
 </sst>
 </file>
@@ -2065,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47979A52-AC7D-48A2-A130-CC6D77928906}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,667 +2359,144 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C36428-63BD-472E-9AEF-E7AD7E6DF397}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
-  <dimension ref="A1:K28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C593A65-72D5-488B-B99F-1E676D8D6A63}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:K28"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4">
-        <v>0</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="4">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="4">
-        <v>3</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="4">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="1">
-        <v>802</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="1">
-        <v>802</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="1">
-        <v>802</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H27" s="1">
-        <v>92000</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3060,6 +2586,664 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView zoomScale="130" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1">
+        <v>802</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="1">
+        <v>802</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="1">
+        <v>802</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="1">
+        <v>92000</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4009,6 +4193,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -4196,14 +4388,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
   <ds:schemaRefs>
@@ -4213,6 +4397,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4228,20 +4428,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
12 Commit - tc task manager 18,19,20
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{70064AC4-793D-43B6-A904-992B3B16F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BDA10CFC-3358-4D3C-832B-E238CCB56768}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{70064AC4-793D-43B6-A904-992B3B16F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F7AE06F3-5937-451C-8555-9B852594AF53}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="16" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,8 @@
     <sheet name="History Cleaner" sheetId="18" r:id="rId17"/>
     <sheet name="Registry Backup Restore" sheetId="19" r:id="rId18"/>
     <sheet name="Startup Application List" sheetId="20" r:id="rId19"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId20"/>
+    <sheet name="Task Scheduler" sheetId="21" r:id="rId20"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId21"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="235">
   <si>
     <t>Email</t>
   </si>
@@ -737,6 +738,18 @@
   </si>
   <si>
     <t>file1.exe</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Refresh</t>
+  </si>
+  <si>
+    <t>MicrosoftEdgeUpdateTaskMachineCore</t>
   </si>
 </sst>
 </file>
@@ -2445,8 +2458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C593A65-72D5-488B-B99F-1E676D8D6A63}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2590,6 +2603,55 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE19630C-EDE5-4BC4-9116-6FE0D3ED4CB9}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
   <dimension ref="A1:K28"/>
   <sheetViews>
@@ -4184,20 +4246,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4389,25 +4451,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
30/12/24 Commit - added software deployment - install uninstall  test cases tc21,22
TC_TM_021_apply_administration_settings_remote_agent_advanced_settings
TC_TM_022_software_deployment_software_and_patch_install_uninstall
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{70064AC4-793D-43B6-A904-992B3B16F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F7AE06F3-5937-451C-8555-9B852594AF53}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{70064AC4-793D-43B6-A904-992B3B16F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{26BA6590-28A6-4A49-B983-1FB7923B5143}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="16" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="17" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,9 @@
     <sheet name="Registry Backup Restore" sheetId="19" r:id="rId18"/>
     <sheet name="Startup Application List" sheetId="20" r:id="rId19"/>
     <sheet name="Task Scheduler" sheetId="21" r:id="rId20"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId21"/>
+    <sheet name="Advanced Settings" sheetId="22" r:id="rId21"/>
+    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId22"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId23"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="279">
   <si>
     <t>Email</t>
   </si>
@@ -750,6 +752,138 @@
   </si>
   <si>
     <t>MicrosoftEdgeUpdateTaskMachineCore</t>
+  </si>
+  <si>
+    <t>Task Reboot Monitoring</t>
+  </si>
+  <si>
+    <t>DHCP Discovery</t>
+  </si>
+  <si>
+    <t>Monitoring and Maintainance</t>
+  </si>
+  <si>
+    <t>Battery Indicator</t>
+  </si>
+  <si>
+    <t>Idle State</t>
+  </si>
+  <si>
+    <t>Config Sync</t>
+  </si>
+  <si>
+    <t>BootLog</t>
+  </si>
+  <si>
+    <t>Usb Mass Storage Logs</t>
+  </si>
+  <si>
+    <t>Screen Saver Logs</t>
+  </si>
+  <si>
+    <t>Enable Vnc Acceptance</t>
+  </si>
+  <si>
+    <t>Sync Task Scheduler</t>
+  </si>
+  <si>
+    <t>Application Log</t>
+  </si>
+  <si>
+    <t>Cpu Utilization Log</t>
+  </si>
+  <si>
+    <t>Write Filter Logs</t>
+  </si>
+  <si>
+    <t>SignalR Monitoring</t>
+  </si>
+  <si>
+    <t>Hardware Logs</t>
+  </si>
+  <si>
+    <t>Enable Agent Debug Logs</t>
+  </si>
+  <si>
+    <t>Download Attempts</t>
+  </si>
+  <si>
+    <t>Location Range</t>
+  </si>
+  <si>
+    <t>Hardware Logs Interval</t>
+  </si>
+  <si>
+    <t>Heart Beat Interval</t>
+  </si>
+  <si>
+    <t>SignalR Connection Path</t>
+  </si>
+  <si>
+    <t>User Level</t>
+  </si>
+  <si>
+    <t>Developer Level</t>
+  </si>
+  <si>
+    <t>/communication/signalr/hubs</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Select New Install Or Uninstall</t>
+  </si>
+  <si>
+    <t>Source Type</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Global Repository</t>
+  </si>
+  <si>
+    <t>NEW INSTALL</t>
+  </si>
+  <si>
+    <t>Repository</t>
+  </si>
+  <si>
+    <t>FDM_HTTP</t>
+  </si>
+  <si>
+    <t>ChromeSetup.exe</t>
+  </si>
+  <si>
+    <t>/quiet</t>
+  </si>
+  <si>
+    <t>New Upload</t>
+  </si>
+  <si>
+    <t>HTTPS</t>
+  </si>
+  <si>
+    <t>$Group$</t>
+  </si>
+  <si>
+    <t>$GROUP$</t>
+  </si>
+  <si>
+    <t>AnyDesk.exe</t>
   </si>
 </sst>
 </file>
@@ -779,7 +913,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -813,11 +947,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -836,6 +983,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2606,8 +2755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE19630C-EDE5-4BC4-9116-6FE0D3ED4CB9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,15 +2797,408 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D193770-0DE9-4AFF-A9CD-47CBE6D06952}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="V2" s="1">
+        <v>6</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="V3" s="1">
+        <v>6</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32692EE9-61EF-4346-8B2E-6D573605C2CE}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:K28"/>
+    <sheetView topLeftCell="A19" zoomScale="130" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3301,6 +3843,110 @@
         <v>3</v>
       </c>
       <c r="K28" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4246,14 +4892,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4262,7 +4900,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -4450,23 +5088,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4474,7 +5104,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4490,4 +5120,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
31/12/24 Commit - added template manager test cases tc_tm_022, tc_tm_023
TC_TM_022_apply_administration_settings_remote_agent_change_vnc_password
TC_TM_023_apply_administration_settings_remote_agent_general_settings
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{70064AC4-793D-43B6-A904-992B3B16F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{26BA6590-28A6-4A49-B983-1FB7923B5143}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{70064AC4-793D-43B6-A904-992B3B16F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{046762F8-8189-4FE3-A120-971BF046F8E8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="17" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="19" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,9 @@
     <sheet name="Task Scheduler" sheetId="21" r:id="rId20"/>
     <sheet name="Advanced Settings" sheetId="22" r:id="rId21"/>
     <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId22"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId23"/>
+    <sheet name="Change VNC Password" sheetId="25" r:id="rId23"/>
+    <sheet name="General Settings" sheetId="26" r:id="rId24"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId25"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="283">
   <si>
     <t>Email</t>
   </si>
@@ -884,6 +886,18 @@
   </si>
   <si>
     <t>AnyDesk.exe</t>
+  </si>
+  <si>
+    <t>VNC Password</t>
+  </si>
+  <si>
+    <t>Server IP Name</t>
+  </si>
+  <si>
+    <t>Port Number</t>
+  </si>
+  <si>
+    <t>winserver.vdi.com</t>
   </si>
 </sst>
 </file>
@@ -3068,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32692EE9-61EF-4346-8B2E-6D573605C2CE}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3194,6 +3208,98 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93683C3E-F6E3-4E2D-A41A-96C24AE51928}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F76283-0284-477C-A0E1-221B144A3917}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="1">
+        <v>443</v>
+      </c>
+      <c r="D2" s="1">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -4892,15 +4998,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -5088,7 +5185,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
@@ -5096,15 +5193,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5122,18 +5220,26 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
31/12/24 Commit - completed tc template manager tc 24,25,26
TC_TM_024_apply_administration_settings_service_management_services
TC_TM_025_apply_administration_settings_service_management_usb_device_manager
TC_TM_026_apply_administration_settings_service_management_user_management
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{70064AC4-793D-43B6-A904-992B3B16F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{046762F8-8189-4FE3-A120-971BF046F8E8}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{70064AC4-793D-43B6-A904-992B3B16F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{ED367099-E704-4955-A35C-2AB029272800}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="19" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="21" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,10 @@
     <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId22"/>
     <sheet name="Change VNC Password" sheetId="25" r:id="rId23"/>
     <sheet name="General Settings" sheetId="26" r:id="rId24"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId25"/>
+    <sheet name="Services" sheetId="27" r:id="rId25"/>
+    <sheet name="USB Device Manager" sheetId="28" r:id="rId26"/>
+    <sheet name="User Management" sheetId="29" r:id="rId27"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId28"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="316">
   <si>
     <t>Email</t>
   </si>
@@ -898,16 +901,123 @@
   </si>
   <si>
     <t>winserver.vdi.com</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Startup Type</t>
+  </si>
+  <si>
+    <t>Microsoft App-V Client</t>
+  </si>
+  <si>
+    <t>VIEW</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Automatic</t>
+  </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>RESTART</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>USB Device Controller Status</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Audio/Video</t>
+  </si>
+  <si>
+    <t>Human Interface</t>
+  </si>
+  <si>
+    <t>Image Devices</t>
+  </si>
+  <si>
+    <t>Mass Storage</t>
+  </si>
+  <si>
+    <t>Printers</t>
+  </si>
+  <si>
+    <t>Smart Card Reader</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Wireless Controllers</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Member Of</t>
+  </si>
+  <si>
+    <t>User Can Not Change The Password</t>
+  </si>
+  <si>
+    <t>Password Never Expires</t>
+  </si>
+  <si>
+    <t>Disable User</t>
+  </si>
+  <si>
+    <t>Add User</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin@123</t>
+  </si>
+  <si>
+    <t>Admin Admin</t>
+  </si>
+  <si>
+    <t>testdata description</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Reset User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -975,10 +1085,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -999,8 +1110,10 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3254,8 +3367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F76283-0284-477C-A0E1-221B144A3917}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3300,6 +3413,422 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287760A5-7A67-48AD-A225-152416471720}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662CFF93-55A6-4800-A79E-B4AD6B76DAB4}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0651430C-B53C-46FF-88EE-C88461C708DA}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5ABB11AE-16C7-4605-8B8B-4BC057ED356E}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{57DEC2C1-E1BE-4A15-9F09-97C5B18BA42B}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{4CC34BA5-97B0-4876-9642-A3C41A474340}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -4998,6 +5527,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -5185,14 +5722,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5203,6 +5732,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5220,22 +5765,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
02/01/25 Commit 3 - Optimized the framework
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4" documentId="8_{8DF9A577-392E-4330-80A0-8413EACD350B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8C0ADCA5-D088-4B82-AE98-56E1EAAAA056}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -3867,7 +3867,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="130" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:H34"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4629,7 +4629,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5768,14 +5768,14 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
06/01/25 Commit excel update
updated usersettings excel row 1
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{F5CB9422-ACA2-418A-B857-EE9F760A117B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A969C5E3-7645-41BF-9742-E5783E4D64A2}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{F5CB9422-ACA2-418A-B857-EE9F760A117B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8DD5B743-46CE-4A5A-BF67-794800466DFE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="23" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -2169,15 +2169,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990357BF-34A2-47B3-BEE2-914E91C537BD}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2187,12 +2187,6 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
-        <f>MasterTemplate</f>
-        <v>AAA_UEM_Automation_Template</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="str">
         <f>MasterTemplate</f>
         <v>AAA_UEM_Automation_Template</v>
       </c>
@@ -3850,7 +3844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7878CC6-FA40-4D94-9C3C-EEB0F9DD79C6}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -5956,6 +5950,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -6143,24 +6154,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6176,28 +6194,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
06/01/25 Commit - added tc
TC_TM_028_apply_security_network_Firewall
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{F5CB9422-ACA2-418A-B857-EE9F760A117B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8DD5B743-46CE-4A5A-BF67-794800466DFE}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{F5CB9422-ACA2-418A-B857-EE9F760A117B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BFC4D08C-BC95-49F0-85A1-95D4CDDFEFC3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="26" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,8 @@
     <sheet name="UserManagement" sheetId="29" r:id="rId27"/>
     <sheet name="WriteFilterOperations" sheetId="32" r:id="rId28"/>
     <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId29"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId30"/>
+    <sheet name="Firewall" sheetId="33" r:id="rId30"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId31"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="348">
   <si>
     <t>Email</t>
   </si>
@@ -1068,6 +1069,39 @@
   </si>
   <si>
     <t>Overlay Settings</t>
+  </si>
+  <si>
+    <t>Select Protocol</t>
+  </si>
+  <si>
+    <t>Program Name</t>
+  </si>
+  <si>
+    <t>Program Path</t>
+  </si>
+  <si>
+    <t>Add Port</t>
+  </si>
+  <si>
+    <t>testname</t>
+  </si>
+  <si>
+    <t>168.128.1</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>UDP</t>
+  </si>
+  <si>
+    <t>Add Program</t>
+  </si>
+  <si>
+    <t>testprogramname</t>
+  </si>
+  <si>
+    <t>C:\\Program Files\\Internet Explorer\\iexplore.exe</t>
   </si>
 </sst>
 </file>
@@ -2171,7 +2205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990357BF-34A2-47B3-BEE2-914E91C537BD}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
@@ -4101,7 +4135,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4436,6 +4470,125 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D8816D-F791-4B8E-A2E9-014CB74557C0}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>AAA_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>AAA_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>AAA_UEM_Automation_Template</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -6165,15 +6318,15 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
06/01/25 Commit - added tc and excel
TC_TM_029_apply_security_network_ProxySettings completed with excel data integration
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{F5CB9422-ACA2-418A-B857-EE9F760A117B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{BFC4D08C-BC95-49F0-85A1-95D4CDDFEFC3}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{F5CB9422-ACA2-418A-B857-EE9F760A117B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D153FEE5-89B0-4E16-861E-86203993D80A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="26" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="26" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,8 @@
     <sheet name="WriteFilterOperations" sheetId="32" r:id="rId28"/>
     <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId29"/>
     <sheet name="Firewall" sheetId="33" r:id="rId30"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId31"/>
+    <sheet name="ProxySettings" sheetId="34" r:id="rId31"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId32"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="352">
   <si>
     <t>Email</t>
   </si>
@@ -1102,6 +1103,18 @@
   </si>
   <si>
     <t>C:\\Program Files\\Internet Explorer\\iexplore.exe</t>
+  </si>
+  <si>
+    <t>Automatically Detect Settings</t>
+  </si>
+  <si>
+    <t>Use Automatic Configuration Script</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>test address</t>
   </si>
 </sst>
 </file>
@@ -4473,8 +4486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D8816D-F791-4B8E-A2E9-014CB74557C0}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4589,6 +4602,56 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1DECF9-04EF-4E5D-8B28-CA02496B720C}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>AAA_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -6103,23 +6166,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -6307,31 +6353,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6347,4 +6386,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
07/01/25 Commit - added tc 30 software restrictions
TC_TM_030_apply_security_network_SoftwareRestriction
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_CBF0CE34DC0A8DC217236375AC32C02EF251D815" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{19D7E1DE-3378-4D7D-8417-9676E0D34222}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{EF6C5A25-BE6E-4CC7-8E77-47FF0D7A62B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5112FBB5-DD04-4772-80A9-24D1F7891426}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="18" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="27" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,8 @@
     <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId29"/>
     <sheet name="Firewall" sheetId="33" r:id="rId30"/>
     <sheet name="ProxySettings" sheetId="34" r:id="rId31"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId32"/>
+    <sheet name="SoftwareRestriction" sheetId="35" r:id="rId32"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId33"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="364">
   <si>
     <t>Email</t>
   </si>
@@ -1115,6 +1116,42 @@
   </si>
   <si>
     <t>35</t>
+  </si>
+  <si>
+    <t>Installation &amp; Uninstallation Restriction</t>
+  </si>
+  <si>
+    <t>Software Restriction</t>
+  </si>
+  <si>
+    <t>Software Application  Name</t>
+  </si>
+  <si>
+    <t>Browser Name</t>
+  </si>
+  <si>
+    <t>Restriction Type</t>
+  </si>
+  <si>
+    <t>Installation &amp; Uninstallation</t>
+  </si>
+  <si>
+    <t>Application Restriction</t>
+  </si>
+  <si>
+    <t>Deny All</t>
+  </si>
+  <si>
+    <t>Browser Restriction</t>
+  </si>
+  <si>
+    <t>Block all downloads</t>
+  </si>
+  <si>
+    <t>chrome.exe</t>
+  </si>
+  <si>
+    <t>Allow All</t>
   </si>
 </sst>
 </file>
@@ -3018,7 +3055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
@@ -4519,7 +4556,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4565,6 +4602,149 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35377E32-F425-41C1-BE62-1D8FE1EF50D9}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -5911,6 +6091,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -6098,24 +6295,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6131,28 +6335,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
08/01/25 Commit - excel update, added tc 31 32
TC_TM_031_apply_security_system_DataWipe
TC_TM_032_apply_security_system_DeployCertificate
cer file
pfx file
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cybercorpkolkata-my.sharepoint.com/personal/prajwal_solanke_sundynetech_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{EF6C5A25-BE6E-4CC7-8E77-47FF0D7A62B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5112FBB5-DD04-4772-80A9-24D1F7891426}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{5C33F4F3-0D11-4F27-98D5-5FC2BC85AE49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="27" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="28" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,9 @@
     <sheet name="Firewall" sheetId="33" r:id="rId30"/>
     <sheet name="ProxySettings" sheetId="34" r:id="rId31"/>
     <sheet name="SoftwareRestriction" sheetId="35" r:id="rId32"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId33"/>
+    <sheet name="DataWipe" sheetId="36" r:id="rId33"/>
+    <sheet name="DeployCertificate" sheetId="37" r:id="rId34"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId35"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="377">
   <si>
     <t>Email</t>
   </si>
@@ -1152,6 +1154,45 @@
   </si>
   <si>
     <t>Allow All</t>
+  </si>
+  <si>
+    <t>File Folder</t>
+  </si>
+  <si>
+    <t>C:\Users\admin\Documents</t>
+  </si>
+  <si>
+    <t>ConnectionName</t>
+  </si>
+  <si>
+    <t>Certificate Type</t>
+  </si>
+  <si>
+    <t>Store Name</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>CER</t>
+  </si>
+  <si>
+    <t>ShradhaCerFile.cer</t>
+  </si>
+  <si>
+    <t>Personal certificates</t>
+  </si>
+  <si>
+    <t>PFX</t>
+  </si>
+  <si>
+    <t>Trusted Publishers</t>
+  </si>
+  <si>
+    <t>FTPS</t>
+  </si>
+  <si>
+    <t>ShradhaPexFile.pfx</t>
   </si>
 </sst>
 </file>
@@ -4605,8 +4646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35377E32-F425-41C1-BE62-1D8FE1EF50D9}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4745,6 +4786,262 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00BFAE6-5FA2-404A-9765-F19A9E04F244}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057ECABA-A180-4964-8A7E-BC5BFBC01DFF}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A7" si="0">MasterTemplate</f>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{A35D947A-2BC5-4099-9C4B-747F5D3367C6}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{00BA1DCF-C9AB-4A75-8424-BF572BD573A9}"/>
+    <hyperlink ref="G6" r:id="rId3" display="admin@123" xr:uid="{4A306E95-E215-4009-A370-8418E7A58552}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{950E95D6-5B15-423F-AC91-5FBC1568A38C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -6298,15 +6595,15 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added tc 33 in task Manager (Integrated Peripheral settings) and excel update
TC_TM_033_apply_security_system_IntegratedPeripheral(
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cybercorpkolkata-my.sharepoint.com/personal/prajwal_solanke_sundynetech_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{5C33F4F3-0D11-4F27-98D5-5FC2BC85AE49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41046594-A447-4095-998D-49316AF8691C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="28" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" firstSheet="28" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,8 @@
     <sheet name="SoftwareRestriction" sheetId="35" r:id="rId32"/>
     <sheet name="DataWipe" sheetId="36" r:id="rId33"/>
     <sheet name="DeployCertificate" sheetId="37" r:id="rId34"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId35"/>
+    <sheet name="IntegratedPeripheral" sheetId="38" r:id="rId35"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId36"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="381">
   <si>
     <t>Email</t>
   </si>
@@ -1193,6 +1194,18 @@
   </si>
   <si>
     <t>ShradhaPexFile.pfx</t>
+  </si>
+  <si>
+    <t>Enable CD DVD</t>
+  </si>
+  <si>
+    <t>Bluetooth Device</t>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t>Disable</t>
   </si>
 </sst>
 </file>
@@ -4825,8 +4838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057ECABA-A180-4964-8A7E-BC5BFBC01DFF}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5042,6 +5055,74 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8B6CF2-BC42-47EC-A29F-5DBA86E0282E}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A4" si="0">MasterTemplate</f>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A23_UEM_Automation_Template</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -6388,20 +6469,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6593,25 +6674,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added TC_TM_036_apply_connectionManagement_Connections_CustomExecutable with excel sheet
TC_TM_036_apply_connectionManagement_Connections_CustomExecutable
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_2FE68CDB74FA199B89411D9221F073A8E281290F" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D5AB3068-4538-4C40-8179-85947BC9A246}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_2FE68CDB74FA199B89411D9221F073A8E281290F" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3D730F05-8094-491D-ACD3-C96668700888}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" firstSheet="29" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" firstSheet="30" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,8 @@
     <sheet name="IntegratedPeripheral" sheetId="38" r:id="rId35"/>
     <sheet name="PortSettings" sheetId="39" r:id="rId36"/>
     <sheet name="CitrixWorkspace" sheetId="40" r:id="rId37"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId38"/>
+    <sheet name="CustomExecutable" sheetId="41" r:id="rId38"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId39"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="403">
   <si>
     <t>Email</t>
   </si>
@@ -1251,6 +1252,24 @@
   </si>
   <si>
     <t>https://192.168.1.23/Citrix/PNAgent/Config.xml</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Create Shortcut On Desktop</t>
+  </si>
+  <si>
+    <t>Auto Start Connection</t>
+  </si>
+  <si>
+    <t>Arguments</t>
+  </si>
+  <si>
+    <t>C:\Applications\AppBusiness.exe</t>
+  </si>
+  <si>
+    <t>testArguments</t>
   </si>
 </sst>
 </file>
@@ -5277,8 +5296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BEC3E4-E5E1-433E-AD96-E993DB0F10E1}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5363,6 +5382,91 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DF793F-8BC4-4006-8A55-542F8FEBAF7E}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A3" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -6709,12 +6813,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6906,16 +7009,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
-  <ds:schemaRefs/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
@@ -6926,17 +7040,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+  <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
optimized the framework and added tc
TC_TM_038_apply_connectionManagement_Connections_RDP completed with excel integration
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_2FE68CDB74FA199B89411D9221F073A8E281290F" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{CEBB4D84-8A6E-4B72-A2CF-710E6907F634}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="11_2FE68CDB74FA199B89411D9221F073A8E281290F" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0C24DB78-9D65-4E6E-BB30-6835EEFF9F70}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" firstSheet="31" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,8 @@
     <sheet name="CitrixWorkspace" sheetId="40" r:id="rId37"/>
     <sheet name="CustomExecutable" sheetId="41" r:id="rId38"/>
     <sheet name="Browser" sheetId="42" r:id="rId39"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId40"/>
+    <sheet name="RDP" sheetId="43" r:id="rId40"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId41"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="450">
   <si>
     <t>Email</t>
   </si>
@@ -1096,9 +1097,6 @@
     <t>Allow All</t>
   </si>
   <si>
-    <t>chrome.exe</t>
-  </si>
-  <si>
     <t>Deny All</t>
   </si>
   <si>
@@ -1289,18 +1287,151 @@
   </si>
   <si>
     <t>Edge</t>
+  </si>
+  <si>
+    <t>IP Host Name</t>
+  </si>
+  <si>
+    <t>Always Ask For Cred</t>
+  </si>
+  <si>
+    <t>Automatic Start</t>
+  </si>
+  <si>
+    <t>Use All Monitors For Remote Session</t>
+  </si>
+  <si>
+    <t>Full Screen</t>
+  </si>
+  <si>
+    <t>Size Of Desktop</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>Display Connection Bar</t>
+  </si>
+  <si>
+    <t>Remote Audio Playback</t>
+  </si>
+  <si>
+    <t>Remote Audio Recording</t>
+  </si>
+  <si>
+    <t>Drives</t>
+  </si>
+  <si>
+    <t>Clipboard</t>
+  </si>
+  <si>
+    <t>Smart Cards</t>
+  </si>
+  <si>
+    <t>Ports</t>
+  </si>
+  <si>
+    <t>PNP Devices</t>
+  </si>
+  <si>
+    <t>Keyboard</t>
+  </si>
+  <si>
+    <t>Program Path File Name</t>
+  </si>
+  <si>
+    <t>Start In Following Folder</t>
+  </si>
+  <si>
+    <t>Connection Speed</t>
+  </si>
+  <si>
+    <t>Reconnect If Connection Dropped</t>
+  </si>
+  <si>
+    <t>Authentication Option</t>
+  </si>
+  <si>
+    <t>Do Not Use RD Gateway</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Automatic Logon</t>
+  </si>
+  <si>
+    <t>192.168.3.138</t>
+  </si>
+  <si>
+    <t>Start Program On Connection</t>
+  </si>
+  <si>
+    <t>vdi.com</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>1024x768</t>
+  </si>
+  <si>
+    <t>High Color(16 bit)</t>
+  </si>
+  <si>
+    <t>True Color(24 bit)</t>
+  </si>
+  <si>
+    <t>Local Resources</t>
+  </si>
+  <si>
+    <t>Do not play</t>
+  </si>
+  <si>
+    <t>Do not record</t>
+  </si>
+  <si>
+    <t>On the remote computer</t>
+  </si>
+  <si>
+    <t>Programs</t>
+  </si>
+  <si>
+    <t>D:\sample\sample.exe</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>LAN(10 Mbps or higher)</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Warn me</t>
+  </si>
+  <si>
+    <t>explorer.exe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1384,9 +1515,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1397,7 +1528,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1410,7 +1541,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1687,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1715,10 +1847,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -1726,32 +1858,32 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -1759,7 +1891,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -1770,19 +1902,30 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4236,7 +4379,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4286,7 +4429,7 @@
         <v>312</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>314</v>
@@ -4313,10 +4456,10 @@
         <v>312</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>315</v>
@@ -4744,7 +4887,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4820,7 +4963,7 @@
         <v>343</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>344</v>
+        <v>449</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>26</v>
@@ -4841,10 +4984,10 @@
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>344</v>
+        <v>212</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>26</v>
@@ -4859,7 +5002,7 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
@@ -4874,7 +5017,7 @@
         <v>196</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -4901,7 +5044,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4910,7 +5053,7 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -4920,10 +5063,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4946,27 +5089,27 @@
         <v>308</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>350</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>351</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>309</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="str">
-        <f t="shared" ref="A2:A7" si="0">MasterTemplate</f>
+        <f t="shared" ref="A2:A8" si="0">MasterTemplate</f>
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4976,13 +5119,13 @@
         <v>314</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>26</v>
@@ -5000,16 +5143,16 @@
         <v>317</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>280</v>
@@ -5024,25 +5167,25 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>314</v>
+        <v>356</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>358</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>280</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>355</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -5057,19 +5200,19 @@
         <v>314</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>280</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -5078,25 +5221,25 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>280</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5111,27 +5254,55 @@
         <v>320</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
-    <hyperlink ref="G5" r:id="rId2" xr:uid="{00000000-0004-0000-2100-000001000000}"/>
-    <hyperlink ref="G6" r:id="rId3" xr:uid="{00000000-0004-0000-2100-000002000000}"/>
-    <hyperlink ref="G7" r:id="rId4" xr:uid="{00000000-0004-0000-2100-000003000000}"/>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
+    <hyperlink ref="G6" r:id="rId2" xr:uid="{00000000-0004-0000-2100-000001000000}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{00000000-0004-0000-2100-000002000000}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{00000000-0004-0000-2100-000003000000}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{0421A459-F154-4D79-9639-94FC8E6EC1FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5158,10 +5329,10 @@
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>361</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -5170,10 +5341,10 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -5182,10 +5353,10 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -5231,25 +5402,25 @@
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>369</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -5334,16 +5505,16 @@
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>388</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>389</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>273</v>
@@ -5355,19 +5526,19 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5376,19 +5547,19 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>396</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -5423,19 +5594,19 @@
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>399</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -5444,19 +5615,19 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5465,10 +5636,10 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>24</v>
@@ -5477,7 +5648,7 @@
         <v>44</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -5489,8 +5660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9CF9A1-DEC6-4E65-B8D9-9D889BEE77EF}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5510,25 +5681,25 @@
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>404</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -5537,13 +5708,13 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>407</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>44</v>
@@ -5564,13 +5735,13 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
@@ -5840,6 +6011,1047 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB8B2B7-7CA9-4C4B-9B22-221B73EA37BC}">
+  <dimension ref="A1:AF10"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AB18" sqref="AB18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>433</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A10" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4455</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4455</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32">
+      <c r="A4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32">
+      <c r="A5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32">
+      <c r="A6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32">
+      <c r="A7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32">
+      <c r="A8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32">
+      <c r="A9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32">
+      <c r="A10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="prajwal@vdi.com" xr:uid="{5100CE7D-5248-4F70-9865-1B61E7AB9DA9}"/>
+    <hyperlink ref="H3" r:id="rId2" display="prajwal@vdi.com" xr:uid="{50CEEA5D-E759-4F05-B140-4B22E66D6D0F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -5851,7 +7063,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>23</v>
@@ -5904,7 +7116,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -5933,7 +7145,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -5948,7 +7160,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G7" s="2">
         <v>2</v>
@@ -5962,7 +7174,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
@@ -5971,13 +7183,13 @@
         <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E8" s="2">
         <v>3</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G8" s="2">
         <v>13</v>
@@ -5991,7 +7203,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
@@ -6000,7 +7212,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -6020,10 +7232,10 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>378</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>26</v>
@@ -6049,16 +7261,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>26</v>
@@ -6078,10 +7290,10 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>26</v>
@@ -6107,16 +7319,16 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>26</v>
@@ -6136,10 +7348,10 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>384</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>26</v>
@@ -6165,16 +7377,16 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>26</v>
@@ -6354,7 +7566,7 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>121</v>
@@ -6389,7 +7601,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>121</v>
@@ -6424,7 +7636,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>126</v>
@@ -6459,13 +7671,13 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>26</v>
@@ -6520,7 +7732,7 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>312</v>
@@ -6546,7 +7758,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>312</v>
@@ -6572,7 +7784,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>312</v>
@@ -6941,6 +8153,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -7128,7 +8349,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
@@ -7136,39 +8357,30 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added new tc TC_TM_039_apply_connectionManagement_Connections_Teradici
TC_TM_039_apply_connectionManagement_Connections_Teradici
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="11_2FE68CDB74FA199B89411D9221F073A8E281290F" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0C24DB78-9D65-4E6E-BB30-6835EEFF9F70}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="11_2FE68CDB74FA199B89411D9221F073A8E281290F" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4EDCECB5-67D7-42BF-ABEF-A5A3A1E4E7E9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" firstSheet="32" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,8 @@
     <sheet name="CustomExecutable" sheetId="41" r:id="rId38"/>
     <sheet name="Browser" sheetId="42" r:id="rId39"/>
     <sheet name="RDP" sheetId="43" r:id="rId40"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId41"/>
+    <sheet name="Teradici" sheetId="44" r:id="rId41"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId42"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="458">
   <si>
     <t>Email</t>
   </si>
@@ -1413,6 +1414,30 @@
   </si>
   <si>
     <t>explorer.exe</t>
+  </si>
+  <si>
+    <t>Host Name</t>
+  </si>
+  <si>
+    <t>Remote work station card</t>
+  </si>
+  <si>
+    <t>Usb Disable</t>
+  </si>
+  <si>
+    <t>Create Shortcut in the start menu</t>
+  </si>
+  <si>
+    <t>Teradici PCoIP</t>
+  </si>
+  <si>
+    <t>vdi</t>
+  </si>
+  <si>
+    <t>Windowed</t>
+  </si>
+  <si>
+    <t>Fullscreen</t>
   </si>
 </sst>
 </file>
@@ -1821,7 +1846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
@@ -6015,7 +6040,7 @@
   <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AB18" sqref="AB18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7052,6 +7077,151 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C85BBD-E301-4B30-9FF9-BA00C2199C89}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A3" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -8153,6 +8323,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8161,7 +8339,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -8349,38 +8527,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
optimized the framework and updated the changes
error fixes

TC_TM_030_apply_security_network_SoftwareRestriction
Cannot locate option with text: explorer.exe

TC_TM_040_apply_connectionManagement_Connections_VMWareview
Cannot locate option with text: 1280x720

TC_TM_050_software_deployment_SoftwarePatchInstallUninstall
Cannot locate option with text: AnyDesk.exe
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cybercorpkolkata-my.sharepoint.com/personal/prajwal_solanke_sundynetech_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="11_2FE68CDB74FA199B89411D9221F073A8E281290F" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4EDCECB5-67D7-42BF-ABEF-A5A3A1E4E7E9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{73E0EE12-0C47-4BBB-BDE4-1459BAAA3C5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" firstSheet="32" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" firstSheet="29" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -41,20 +41,21 @@
     <sheet name="USBDeviceManager" sheetId="28" r:id="rId26"/>
     <sheet name="UserManagement" sheetId="29" r:id="rId27"/>
     <sheet name="WriteFilterOperations" sheetId="32" r:id="rId28"/>
-    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId29"/>
-    <sheet name="Firewall" sheetId="33" r:id="rId30"/>
-    <sheet name="ProxySettings" sheetId="34" r:id="rId31"/>
-    <sheet name="SoftwareRestriction" sheetId="35" r:id="rId32"/>
-    <sheet name="DataWipe" sheetId="36" r:id="rId33"/>
-    <sheet name="DeployCertificate" sheetId="37" r:id="rId34"/>
-    <sheet name="IntegratedPeripheral" sheetId="38" r:id="rId35"/>
-    <sheet name="PortSettings" sheetId="39" r:id="rId36"/>
-    <sheet name="CitrixWorkspace" sheetId="40" r:id="rId37"/>
-    <sheet name="CustomExecutable" sheetId="41" r:id="rId38"/>
-    <sheet name="Browser" sheetId="42" r:id="rId39"/>
-    <sheet name="RDP" sheetId="43" r:id="rId40"/>
-    <sheet name="Teradici" sheetId="44" r:id="rId41"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId42"/>
+    <sheet name="Firewall" sheetId="33" r:id="rId29"/>
+    <sheet name="ProxySettings" sheetId="34" r:id="rId30"/>
+    <sheet name="SoftwareRestriction" sheetId="35" r:id="rId31"/>
+    <sheet name="DataWipe" sheetId="36" r:id="rId32"/>
+    <sheet name="DeployCertificate" sheetId="37" r:id="rId33"/>
+    <sheet name="IntegratedPeripheral" sheetId="38" r:id="rId34"/>
+    <sheet name="PortSettings" sheetId="39" r:id="rId35"/>
+    <sheet name="CitrixWorkspace" sheetId="40" r:id="rId36"/>
+    <sheet name="CustomExecutable" sheetId="41" r:id="rId37"/>
+    <sheet name="Browser" sheetId="42" r:id="rId38"/>
+    <sheet name="RDP" sheetId="43" r:id="rId39"/>
+    <sheet name="Teradici" sheetId="44" r:id="rId40"/>
+    <sheet name="VMWareview" sheetId="45" r:id="rId41"/>
+    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId42"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId43"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="471">
   <si>
     <t>Email</t>
   </si>
@@ -1413,9 +1414,6 @@
     <t>Warn me</t>
   </si>
   <si>
-    <t>explorer.exe</t>
-  </si>
-  <si>
     <t>Host Name</t>
   </si>
   <si>
@@ -1438,6 +1436,48 @@
   </si>
   <si>
     <t>Fullscreen</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Application or Desktop Name</t>
+  </si>
+  <si>
+    <t>Smart Card Pin</t>
+  </si>
+  <si>
+    <t>Connect Usb On Startup</t>
+  </si>
+  <si>
+    <t>Connect Usb On Insert</t>
+  </si>
+  <si>
+    <t>Non Interactive</t>
+  </si>
+  <si>
+    <t>Reconnect Behaviour</t>
+  </si>
+  <si>
+    <t>VMW Protocol</t>
+  </si>
+  <si>
+    <t>Desktop Name</t>
+  </si>
+  <si>
+    <t>chrome.exe</t>
+  </si>
+  <si>
+    <t>Reconnect automatically to open applications</t>
+  </si>
+  <si>
+    <t>RDP protocol setting</t>
+  </si>
+  <si>
+    <t>PDF Viewer</t>
+  </si>
+  <si>
+    <t>Citrix Workspace</t>
   </si>
 </sst>
 </file>
@@ -4400,130 +4440,117 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>306</v>
+        <v>50</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>307</v>
+        <v>252</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>308</v>
+        <v>250</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="str">
         <f>MasterTemplate</f>
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>314</v>
+        <v>326</v>
+      </c>
+      <c r="D2" s="1">
+        <v>8765</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>316</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="str">
         <f>MasterTemplate</f>
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>314</v>
+        <v>328</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4433</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>316</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="str">
         <f>MasterTemplate</f>
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>312</v>
+        <v>330</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>319</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>320</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>321</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>44</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -4739,125 +4766,6 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="str">
-        <f>MasterTemplate</f>
-        <v>A101_UEM_Automation_Template</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D2" s="1">
-        <v>8765</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="str">
-        <f>MasterTemplate</f>
-        <v>A101_UEM_Automation_Template</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D3" s="1">
-        <v>4433</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="str">
-        <f>MasterTemplate</f>
-        <v>A101_UEM_Automation_Template</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4907,12 +4815,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4988,7 +4896,7 @@
         <v>343</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>449</v>
+        <v>469</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>26</v>
@@ -5012,7 +4920,7 @@
         <v>344</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>212</v>
+        <v>470</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>26</v>
@@ -5050,7 +4958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -5086,7 +4994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -5334,7 +5242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -5402,7 +5310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -5507,7 +5415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BEC3E4-E5E1-433E-AD96-E993DB0F10E1}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -5596,7 +5504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DF793F-8BC4-4006-8A55-542F8FEBAF7E}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -5681,7 +5589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9CF9A1-DEC6-4E65-B8D9-9D889BEE77EF}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -5790,252 +5698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P4"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" customWidth="1"/>
-    <col min="16" max="16" width="24.140625" customWidth="1"/>
-    <col min="17" max="17" width="19.5703125" customWidth="1"/>
-    <col min="18" max="18" width="5" customWidth="1"/>
-    <col min="19" max="19" width="18.42578125" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" customWidth="1"/>
-    <col min="22" max="23" width="24.28515625" customWidth="1"/>
-    <col min="24" max="24" width="36.7109375" customWidth="1"/>
-    <col min="25" max="25" width="21.5703125" customWidth="1"/>
-    <col min="26" max="26" width="23.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="1" t="str">
-        <f>MasterTemplate</f>
-        <v>A101_UEM_Automation_Template</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="1">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="1" t="str">
-        <f>MasterTemplate</f>
-        <v>A101_UEM_Automation_Template</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="1" t="str">
-        <f>MasterTemplate</f>
-        <v>A101_UEM_Automation_Template</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB8B2B7-7CA9-4C4B-9B22-221B73EA37BC}">
   <dimension ref="A1:AF10"/>
   <sheetViews>
@@ -7076,12 +6739,257 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" customWidth="1"/>
+    <col min="16" max="16" width="24.140625" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" customWidth="1"/>
+    <col min="18" max="18" width="5" customWidth="1"/>
+    <col min="19" max="19" width="18.42578125" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" customWidth="1"/>
+    <col min="21" max="21" width="19.5703125" customWidth="1"/>
+    <col min="22" max="23" width="24.28515625" customWidth="1"/>
+    <col min="24" max="24" width="36.7109375" customWidth="1"/>
+    <col min="25" max="25" width="21.5703125" customWidth="1"/>
+    <col min="26" max="26" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="1">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C85BBD-E301-4B30-9FF9-BA00C2199C89}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7108,7 +7016,7 @@
         <v>386</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>32</v>
@@ -7120,16 +7028,16 @@
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>451</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>452</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>397</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>398</v>
@@ -7144,13 +7052,13 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
@@ -7174,7 +7082,7 @@
         <v>44</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -7183,13 +7091,13 @@
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
@@ -7213,7 +7121,7 @@
         <v>44</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -7221,7 +7129,335 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17A79F0-B263-4E61-8CAF-743040795E27}">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A3" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -8323,14 +8559,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8339,7 +8567,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -8527,30 +8755,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added tc TC_TM_041_apply_VMViewGlobalSettings and fixed changes according to 3.56
TC_TM_041_apply_VMViewGlobalSettings
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cybercorpkolkata-my.sharepoint.com/personal/prajwal_solanke_sundynetech_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73E0EE12-0C47-4BBB-BDE4-1459BAAA3C5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{E2D6B881-A3D2-4649-8872-7E2B39C8D339}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7FF69728-2B97-42CD-AA34-172BB3BC9F69}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" firstSheet="29" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" firstSheet="36" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -54,8 +54,9 @@
     <sheet name="RDP" sheetId="43" r:id="rId39"/>
     <sheet name="Teradici" sheetId="44" r:id="rId40"/>
     <sheet name="VMWareview" sheetId="45" r:id="rId41"/>
-    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId42"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId43"/>
+    <sheet name="VMViewGlobalSettings" sheetId="47" r:id="rId42"/>
+    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId43"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId44"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="481">
   <si>
     <t>Email</t>
   </si>
@@ -1478,6 +1479,36 @@
   </si>
   <si>
     <t>Citrix Workspace</t>
+  </si>
+  <si>
+    <t>Unauthenticated Access</t>
+  </si>
+  <si>
+    <t>Hide Client After Launch</t>
+  </si>
+  <si>
+    <t>Allow H264 Decoding</t>
+  </si>
+  <si>
+    <t>Allow High Color Accuracy</t>
+  </si>
+  <si>
+    <t>Configure SSL</t>
+  </si>
+  <si>
+    <t>Network Condition</t>
+  </si>
+  <si>
+    <t>Never connect to untrusted server</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>Do not verify server identity certificates</t>
+  </si>
+  <si>
+    <t>Poor</t>
   </si>
 </sst>
 </file>
@@ -4819,7 +4850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -7133,8 +7164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17A79F0-B263-4E61-8CAF-743040795E27}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7326,6 +7357,101 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C7C9D1-B1C6-4779-843D-3E1066D897DE}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A3" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -7457,12 +7583,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8212,6 +8338,30 @@
       </c>
       <c r="H34" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="str">
+        <f t="shared" ref="A36" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -8559,15 +8709,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -8755,6 +8896,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -8764,13 +8914,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -8778,15 +8928,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
optimized, saperated pages with objects , added tc
TC_TM_042_apply_remoteOperationTool_DisableClient
TC_TM_043_apply_remoteOperationTool_LockComputer
TC_TM_044_apply_remoteOperationTool_LogOff
TC_TM_045_apply_remoteOperationTool_Restart
TC_TM_046_apply_remoteOperationTool_SendMessageToClient
TC_TM_047_apply_remoteOperationTool_ServiceMode
TC_TM_048_apply_remoteOperationTool_ShutDown
TC_TM_049_apply_remoteOperationTool_SynchroniseInventory
TC_TM_050_apply_remoteOperationTool_WakeOnLan
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{E2D6B881-A3D2-4649-8872-7E2B39C8D339}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7FF69728-2B97-42CD-AA34-172BB3BC9F69}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="8_{E2D6B881-A3D2-4649-8872-7E2B39C8D339}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{635CE44D-9F1C-44B3-90FA-F1B8B65C7050}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" firstSheet="36" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8550" firstSheet="47" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -55,8 +55,17 @@
     <sheet name="Teradici" sheetId="44" r:id="rId40"/>
     <sheet name="VMWareview" sheetId="45" r:id="rId41"/>
     <sheet name="VMViewGlobalSettings" sheetId="47" r:id="rId42"/>
-    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId43"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId44"/>
+    <sheet name="DisableClient" sheetId="48" r:id="rId43"/>
+    <sheet name="LockComputer" sheetId="49" r:id="rId44"/>
+    <sheet name="LogOff" sheetId="50" r:id="rId45"/>
+    <sheet name="Restart" sheetId="51" r:id="rId46"/>
+    <sheet name="SendMessageToClient" sheetId="52" r:id="rId47"/>
+    <sheet name="ServiceMode" sheetId="53" r:id="rId48"/>
+    <sheet name="ShutDown" sheetId="54" r:id="rId49"/>
+    <sheet name="SynchroniseInventory" sheetId="55" r:id="rId50"/>
+    <sheet name="WakeOnLan" sheetId="56" r:id="rId51"/>
+    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId52"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId53"/>
   </sheets>
   <definedNames>
     <definedName name="MasterTemplate">Template!$A$2</definedName>
@@ -66,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="495">
   <si>
     <t>Email</t>
   </si>
@@ -1509,18 +1518,74 @@
   </si>
   <si>
     <t>Poor</t>
+  </si>
+  <si>
+    <t>Disable Client Save</t>
+  </si>
+  <si>
+    <t>Lock Computer Save</t>
+  </si>
+  <si>
+    <t>Importance</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Message from prajwal</t>
+  </si>
+  <si>
+    <t>5 Minute</t>
+  </si>
+  <si>
+    <t>Disabled Service Mode</t>
+  </si>
+  <si>
+    <t>Service Mode</t>
+  </si>
+  <si>
+    <t>Enabled Service Mode</t>
+  </si>
+  <si>
+    <t>Shut Down</t>
+  </si>
+  <si>
+    <t>Inventory Sync</t>
+  </si>
+  <si>
+    <t>Hardware &amp; Software Inventory(Windows)</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Wake On Lan Save</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1611,9 +1676,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1624,7 +1689,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1637,8 +1702,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7360,8 +7427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C7C9D1-B1C6-4779-843D-3E1066D897DE}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7452,129 +7519,33 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589242E6-89E1-4CF1-B175-9A33B7D61751}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="str">
-        <f>MasterTemplate</f>
+        <f t="shared" ref="A2" si="0">MasterTemplate</f>
         <v>A101_UEM_Automation_Template</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="str">
-        <f>MasterTemplate</f>
-        <v>A101_UEM_Automation_Template</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="str">
-        <f>MasterTemplate</f>
-        <v>A101_UEM_Automation_Template</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -7584,784 +7555,276 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
-  <dimension ref="A1:K36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BCCE91-3E04-4E68-A502-564F866F8581}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="2">
-        <v>0</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="E8" s="2">
-        <v>3</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="G8" s="2">
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="1">
-        <v>802</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="1">
-        <v>802</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="1">
-        <v>802</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H27" s="1">
-        <v>92000</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="5" t="s">
+      <c r="B1" s="5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416F9061-7B84-4B25-A46A-D44F915B18A6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1" t="str">
-        <f t="shared" ref="A36" si="0">MasterTemplate</f>
-        <v>A101_UEM_Automation_Template</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>480</v>
+      <c r="B1" s="5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1B9DE4-3151-4432-9050-7A575CBAECD4}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0B3002-D4BA-43F4-B58D-44D7D7E96CE8}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBA058F-608D-4D6F-B80F-3867385F0F21}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A5" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8495A8D-3D6D-4F6B-8682-A2EE450B8100}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -8438,6 +7901,1006 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E464DC-FA47-4F2C-8724-594CCBF1CB82}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A3" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>493</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA31968F-3F48-4A6C-9F66-029EF92AC4A2}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="str">
+        <f>MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="G8" s="2">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1">
+        <v>802</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1">
+        <v>802</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1">
+        <v>802</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27" s="1">
+        <v>92000</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="str">
+        <f t="shared" ref="A36" si="0">MasterTemplate</f>
+        <v>A101_UEM_Automation_Template</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -8709,6 +9172,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -8896,26 +9376,19 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
-  <ds:schemaRefs/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
@@ -8926,17 +9399,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
+  <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>